<commit_message>
merice plages update contrainte
</commit_message>
<xml_diff>
--- a/FOAD/Merise/Exercises/plages.xlsx
+++ b/FOAD/Merise/Exercises/plages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jonat\Documents\GitHub\CRM\CDA_2005\FOAD\Merise\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73E4448-E08B-4FA2-A656-F5F9D833C46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8235E9E9-95B1-4C4E-8EEB-7281847EB3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Entité</t>
   </si>
@@ -101,31 +101,6 @@
   </si>
   <si>
     <t>numerique(2)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">es-que une ville peu avoir plusieurs plage? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reponse client "oui"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Combien de touristes en moyen avez-vous dans les villes? Quel est la longueur maximum d'une de vos plages? Comment nommé vous vos plages?</t>
-    </r>
   </si>
   <si>
     <t>obligatoire</t>
@@ -138,17 +113,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,6 +172,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ADC5A67-E43C-4200-A454-7220997E9655}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6507480" y="228600"/>
+          <a:ext cx="2461260" cy="2004060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>es-que une ville peu avoir plusieurs plage?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Reponse client "oui". </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Combien de touristes en moyen avez-vous dans les villes? </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Quel est la longueur maximum d'une de vos plages?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Comment nommé vous vos plages?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +543,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,9 +594,7 @@
       <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -541,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -562,7 +631,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -577,10 +646,10 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -598,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -608,12 +677,15 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -626,6 +698,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
merice plages update id, attention manque d'info
</commit_message>
<xml_diff>
--- a/FOAD/Merise/Exercises/plages.xlsx
+++ b/FOAD/Merise/Exercises/plages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jonat\Documents\GitHub\CRM\CDA_2005\FOAD\Merise\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8235E9E9-95B1-4C4E-8EEB-7281847EB3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4752414D-1C4A-4E3E-8AF2-7575724BCF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,12 +150,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,7 +543,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,28 +555,28 @@
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -592,12 +592,12 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -612,10 +612,10 @@
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -633,10 +633,10 @@
       <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -651,10 +651,10 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -672,10 +672,10 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">

</xml_diff>